<commit_message>
[IMP] Adjust Output Tax Report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_output_tax.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_output_tax.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Output Tax Report" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t xml:space="preserve">Output Tax Report</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t xml:space="preserve">Taxbranch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run By</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run Date</t>
   </si>
   <si>
     <t xml:space="preserve">Tax Invoice</t>
@@ -77,9 +83,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="#,###.00"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -187,12 +195,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -200,8 +208,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -240,11 +252,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -329,178 +345,210 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.3979591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="2" width="17.3979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="17.3979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="17.3979591836735"/>
-    <col collapsed="false" hidden="false" max="12" min="8" style="2" width="17.3979591836735"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="4" width="17.3979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="5" width="17.3979591836735"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="2" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="4" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="8" style="2" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="13" style="5" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="6" width="17.4"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+    <row r="1" s="8" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
       <c r="L2" s="0"/>
       <c r="M2" s="0"/>
       <c r="N2" s="0"/>
       <c r="O2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
       <c r="L4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
       <c r="L5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="D8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="E8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="F8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="G8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="K6" s="13" t="s">
+      <c r="H8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="I8" s="15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
+      <c r="J8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="L8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="B9" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L9"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.3" right="0.3" top="0.609722222222222" bottom="0.370138888888889" header="0.511805555555555" footer="0.1"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter>&amp;L&amp;8 2018-02-20 09:37:39&amp;R&amp;8&amp;P / &amp;N</oddFooter>

</xml_diff>

<commit_message>
[ENH] pabi_account_report, fix output_tax report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_output_tax.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_output_tax.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t xml:space="preserve">Output Tax Report</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number (preprint)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number (invoice_nuber</t>
   </si>
   <si>
     <t xml:space="preserve">Number</t>
@@ -345,23 +351,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D:D"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="25.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="29.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="4" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="8" style="2" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="13" style="5" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="6" width="17.4"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="3" min="2" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="21.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="29.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="4" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="10" style="2" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="5" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="6" width="17.4"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -376,13 +383,15 @@
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -391,10 +400,12 @@
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
-      <c r="L2" s="0"/>
-      <c r="M2" s="0"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
       <c r="N2" s="0"/>
       <c r="O2" s="0"/>
+      <c r="P2" s="0"/>
+      <c r="Q2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
@@ -410,10 +421,12 @@
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
       <c r="N3" s="12"/>
       <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
@@ -429,7 +442,9 @@
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
-      <c r="L4" s="0"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
@@ -445,15 +460,17 @@
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
-      <c r="L5" s="0"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="14"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
+      <c r="D6" s="14"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
@@ -461,7 +478,9 @@
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
-      <c r="L6" s="0"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
@@ -475,78 +494,88 @@
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
-      <c r="L7" s="0"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="15" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="15"/>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="F8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="G8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="H8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="I8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="J8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="K8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="15" t="s">
+      <c r="L8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="M8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="N8" s="15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="17" t="s">
+      <c r="C9" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="D9" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>20</v>
+      </c>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="A8:D8"/>
     <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:I8"/>
     <mergeCell ref="J8:J9"/>
     <mergeCell ref="K8:K9"/>
     <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="N8:N9"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.3" right="0.3" top="0.609722222222222" bottom="0.370138888888889" header="0.511805555555555" footer="0.1"/>

</xml_diff>